<commit_message>
Enhance car data processing and add 2025 models
Expanded the data pipeline in 1_preprocess.ipynb to generate new CSVs with additional identifiers, and updated parsing logic to handle these. Added and updated CSV files to include new 2025 vehicle models and variants across multiple brands and types. Introduced new .do scripts for data cleaning and simulations, and removed obsolete scripts.
</commit_message>
<xml_diff>
--- a/interm_data/CM_auctions/auction17.xlsx
+++ b/interm_data/CM_auctions/auction17.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yaleedu-my.sharepoint.com/personal/lucas_schmitz_yale_edu/Documents/GitHub/2nd-year-paper/interm_data/CM_auctions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_3FAD378A5B005B30E7F83411595ED87656C9D80F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{869BBF9B-EAC6-403B-99C0-EB91243F0E19}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_3FAD378A5B005B30E7F83411595ED87656C9D80F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CCEDF9E-EB71-4C22-9551-8C5B4EAC5D26}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1706,6 +1706,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2000,7 +2004,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.21875" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
     <col min="3" max="3" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>